<commit_message>
CDS test cases for Experimental Strategy and File Type filters
</commit_message>
<xml_diff>
--- a/InputFiles/TC02_CDS_Filter_ExprStrtgies-MethylationArray.xlsx
+++ b/InputFiles/TC02_CDS_Filter_ExprStrtgies-MethylationArray.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sohilz2\Commons_Automation\InputFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\epishinavv\git\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4390109B-F7B1-46C3-8A49-A7C7D8D3C88D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E411F2AB-F084-4C6D-B393-2855CEBEF65F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-105" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="startup" sheetId="1" r:id="rId1"/>
@@ -48,80 +48,74 @@
     <t>TabName</t>
   </si>
   <si>
-    <t>CasesTab</t>
-  </si>
-  <si>
     <t>SamplesTab</t>
   </si>
   <si>
     <t>FilesTab</t>
   </si>
   <si>
-    <t>TC02_CDS_Filter_ExprStrtgies-MethylationArray_Neo4jData.xlsx</t>
-  </si>
-  <si>
-    <t>TC02_CDS_Filter_ExprStrtgies-MethylationArray_WebData.xlsx</t>
+    <t>ParticipantsTab</t>
   </si>
   <si>
     <t>MATCH (s:study)&lt;--(p:participant)
 OPTIONAL MATCH (p)&lt;--(samp:sample)
+MATCH (samp)&lt;--(f:file)
 OPTIONAL MATCH (p)&lt;--(diag:diagnosis)
-OPTIONAL MATCH (samp)&lt;--(f:file)
 WITH DISTINCT samp,diag,s,p,f
-WHERE s.experimental_strategy_and_data_subtypes in ["Methylation Array"]
+WHERE f.experimental_strategy_and_data_subtypes in ["Methylation Array"]
 RETURN
     count(distinct s) AS Studies,
-    count(distinct diag.primary_diagnosis) AS `Disease Sites`,
     count(distinct p) AS Participants,
     count(distinct samp) AS Samples,
     count(distinct f) AS `Files`</t>
   </si>
   <si>
+    <t>TC02_CDS_Filter_ExprStrtgies-MethylationArray_Neo4jData.xlsx</t>
+  </si>
+  <si>
+    <t>TC02_CDS_Filter_ExprStrtgies-MethylationArray_WebData.xlsx</t>
+  </si>
+  <si>
+    <t>MATCH (s:study)&lt;--(p:participant)&lt;--(samp:sample)
+MATCH (samp)&lt;--(f:file)
+WHERE f.experimental_strategy_and_data_subtypes in ["Methylation Array"]
+WITH p,s,samp,COLLECT(DISTINCT samp.sample_tumor_status) as tumor
+RETURN  
+ coalesce(samp.sample_id, '') as `Sample ID`,
+ coalesce(p.participant_id,'') as `Participant ID`,
+ coalesce(s.study_name, '') as `Study Name`,
+ coalesce(s.phs_accession,'') as `Accession`,
+ coalesce(samp.sample_tumor_status,'') as `Tumor`,
+coalesce(samp.sample_type,'') as `Analyte Type`
+ORDER By samp.sample_id LIMIT 100</t>
+  </si>
+  <si>
     <t>MATCH (s:study)&lt;--(p:participant)
-WHERE s.experimental_strategy_and_data_subtypes in ["Methylation Array"]
 OPTIONAL MATCH (p)&lt;--(samp:sample)
-OPTIONAL MATCH (p)&lt;--(diag:diagnosis)
-OPTIONAL MATCH (samp)&lt;--(f:file)
-WITH DISTINCT p,s,samp,f,diag
+MATCH (samp)&lt;--(f:file)
+WHERE f.experimental_strategy_and_data_subtypes in ["Methylation Array"]
+WITH p, s, collect(distinct samp.sample_id) as samp
+RETURN   
+ coalesce(p.participant_id,'') as `Participant ID`,
+ coalesce(s.study_name, '') as `Study Name`,
+ coalesce(s.phs_accession,'') as `Accession`,
+ coalesce(p.gender,'') as `Gender`,
+ coalesce(apoc.text.join(samp, ','), '') as `Samples`
+ORDER By p.participant_id LIMIT 100</t>
+  </si>
+  <si>
+    <t>MATCH (s:study)&lt;--(p:participant)&lt;--(samp:sample)
+MATCH (samp)&lt;--(f:file)
+WHERE f.experimental_strategy_and_data_subtypes in ["Methylation Array"]
+WITH f,p,s,samp,COLLECT(DISTINCT samp.sample_tumor_status) as tumor
 RETURN 
     coalesce(f.file_name, '') as `File Name`,
     coalesce(s.study_name, '') as `Study Name`,
     coalesce(s.phs_accession,'') as `Accession`,
-    coalesce(p.participant_id,'') as `Subject ID`,
+    coalesce(p.participant_id,'') as `Participant ID`,
     coalesce(samp.sample_id, '') as `Sample ID`,
     coalesce(f.file_type, '') as `File Type`
-   ORDER By f.file_name</t>
-  </si>
-  <si>
-    <t>MATCH (s:study)&lt;--(p:participant)
-WHERE s.experimental_strategy_and_data_subtypes in ["Methylation Array"]
-OPTIONAL MATCH (p)&lt;--(samp:sample)
-OPTIONAL MATCH (p)&lt;--(diag:diagnosis)
-OPTIONAL MATCH (samp)&lt;--(f:file)
-WITH DISTINCT samp,diag,s,p
-RETURN  
- coalesce(samp.sample_id, '') as `Sample ID` ,
- coalesce(s.study_name, '') as `Study Name`,
- coalesce(s.phs_accession,'') as `Accession`,
- coalesce(samp.sample_tumor_status,'') as `Tumor`,
-coalesce(samp.sample_type,'') as `Analyte Type`
-ORDER By samp.sample_id</t>
-  </si>
-  <si>
-    <t>MATCH (s:study)&lt;--(p:participant)
-WHERE s.experimental_strategy_and_data_subtypes in ["Methylation Array"]
-OPTIONAL MATCH (p)&lt;--(samp:sample)
-OPTIONAL MATCH (p)&lt;--(diag:diagnosis)
-OPTIONAL MATCH (samp)&lt;--(f:file)
-WITH DISTINCT samp,diag,s,p
-RETURN  
- coalesce(p.participant_id,'') as `Case ID`,
- coalesce(s.study_name, '') as `Study Name`,
- coalesce(s.phs_accession,'') as `Accession`,
- coalesce(p.gender,'') as `Gender`,
- coalesce(samp.sample_anatomic_site,'') as `Site`,
- coalesce(samp.sample_id, '') as `Samples`
- ORDER By p.participant_id</t>
+ORDER By f.file_name LIMIT 100</t>
   </si>
 </sst>
 </file>
@@ -504,18 +498,18 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="75.77734375" customWidth="1"/>
-    <col min="4" max="4" width="59.88671875" customWidth="1"/>
-    <col min="5" max="5" width="56.88671875" customWidth="1"/>
+    <col min="1" max="1" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="75.7265625" customWidth="1"/>
+    <col min="4" max="4" width="70.26953125" customWidth="1"/>
+    <col min="5" max="5" width="63.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -532,62 +526,62 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="265.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="186" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="186" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="186" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
     </row>
-    <row r="3" spans="1:5" ht="249.6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="234" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C6" s="1"/>
     </row>
   </sheetData>

</xml_diff>